<commit_message>
Read From Excel and Saves new Moduled and Filtered info in a new EXCEL
</commit_message>
<xml_diff>
--- a/DagiCaliburn/bin/Debug/Data.xlsx
+++ b/DagiCaliburn/bin/Debug/Data.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t xml:space="preserve">Type</t>
   </si>
@@ -41,10 +41,61 @@
     <t xml:space="preserve">Thoughts</t>
   </si>
   <si>
-    <t xml:space="preserve">Fully Parsed</t>
+    <t xml:space="preserve">Fully Parsed ? </t>
   </si>
   <si>
     <t xml:space="preserve">Errors while Parsing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Team Leader</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jonnyfekadu@yahoo.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yohanes Fekadu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">University</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hackathon experience ?Tell us why you want to participate on Ethiopia Hack </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TM (Yohanes Fekadu)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">daginegussu@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dagmawi Negussu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">THIS APPLICANT HAS COMPETED BEFORE. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">bekijohn@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bereket Yohannes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Individual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chalakebek@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kebek Chala</t>
+  </si>
+  <si>
+    <t xml:space="preserve">College</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind and entrepreneurs! We have done some projects on our own. </t>
   </si>
 </sst>
 </file>
@@ -114,8 +165,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyFill="1" applyAlignment="0">
       <alignment/>
       <protection locked="1"/>
@@ -137,41 +192,144 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
+      <c r="L1" s="5"/>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2">
+        <v>43807.877037037</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2">
+        <v>932184139</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K2"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3">
+        <v>937886725</v>
+      </c>
+      <c r="J3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4">
+        <v>912345678</v>
+      </c>
+      <c r="J4" t="b">
+        <v>1</v>
+      </c>
+      <c r="K4"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="4">
+        <v>43803.9137384259</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5">
+        <v>932184137</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Main Things Work. Done for the Night
</commit_message>
<xml_diff>
--- a/DagiCaliburn/bin/Debug/Data.xlsx
+++ b/DagiCaliburn/bin/Debug/Data.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
   <si>
     <t xml:space="preserve">Type</t>
   </si>
@@ -71,10 +71,7 @@
     <t xml:space="preserve">daginegussu@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Dagmawi Negussu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">THIS APPLICANT HAS COMPETED BEFORE. </t>
+    <t xml:space="preserve">Name Parsing Error. THIS APPLICANT HAS COMPETED BEFORE. Only 2 attributes Entered.</t>
   </si>
   <si>
     <t xml:space="preserve">bekijohn@gmail.com</t>
@@ -96,6 +93,9 @@
   </si>
   <si>
     <t xml:space="preserve">ind and entrepreneurs! We have done some projects on our own. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email Parsing Error. Name Parsing Error. </t>
   </si>
 </sst>
 </file>
@@ -111,7 +111,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -125,18 +125,42 @@
     </fill>
     <fill>
       <patternFill patternType="none">
-        <fgColor rgb="F4EFEF"/>
+        <fgColor rgb="E1FF00"/>
         <bgColor indexed="0"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="F4EFEF"/>
+        <fgColor rgb="E1FF00"/>
+        <bgColor indexed="0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FF0000"/>
+        <bgColor indexed="0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0000"/>
+        <bgColor indexed="0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C4C4C4"/>
+        <bgColor indexed="0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C4C4C4"/>
         <bgColor indexed="0"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -161,17 +185,63 @@
         <color indexed="0"/>
       </diagonal>
     </border>
+    <border>
+      <left>
+        <color indexed="0"/>
+      </left>
+      <right>
+        <color indexed="0"/>
+      </right>
+      <top>
+        <color indexed="0"/>
+      </top>
+      <bottom>
+        <color indexed="0"/>
+      </bottom>
+      <diagonal>
+        <color indexed="0"/>
+      </diagonal>
+    </border>
+    <border>
+      <left>
+        <color indexed="0"/>
+      </left>
+      <right>
+        <color indexed="0"/>
+      </right>
+      <top>
+        <color indexed="0"/>
+      </top>
+      <bottom>
+        <color indexed="0"/>
+      </bottom>
+      <diagonal>
+        <color indexed="0"/>
+      </diagonal>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="0"/>
+  <cellXfs count="12">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyFill="1" applyAlignment="0">
+      <alignment/>
+      <protection locked="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyFill="1" applyAlignment="0">
+      <alignment/>
+      <protection locked="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyFill="1" applyAlignment="0">
       <alignment/>
       <protection locked="1"/>
     </xf>
@@ -192,40 +262,40 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="5"/>
+      <c r="L1" s="11"/>
     </row>
     <row r="2">
       <c r="A2" t="s">
@@ -261,23 +331,24 @@
       <c r="K2"/>
     </row>
     <row r="3">
-      <c r="A3" t="s">
+      <c r="A3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B3" s="4"/>
+      <c r="C3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="K3" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="E3">
-        <v>937886725</v>
-      </c>
-      <c r="J3" t="b">
-        <v>0</v>
-      </c>
-      <c r="K3" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="4">
@@ -285,10 +356,10 @@
         <v>17</v>
       </c>
       <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
         <v>21</v>
-      </c>
-      <c r="D4" t="s">
-        <v>22</v>
       </c>
       <c r="E4">
         <v>912345678</v>
@@ -300,36 +371,103 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="4">
-        <v>43803.9137384259</v>
+        <v>11</v>
+      </c>
+      <c r="B5" s="8">
+        <v>43807.877037037</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="E5">
-        <v>932184137</v>
+        <v>932184139</v>
       </c>
       <c r="F5" t="s">
         <v>14</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K5"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6"/>
+      <c r="D6" s="3"/>
+      <c r="E6">
+        <v>937886725</v>
+      </c>
+      <c r="J6" t="b">
+        <v>0</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7">
+        <v>945678</v>
+      </c>
+      <c r="J7" t="b">
+        <v>1</v>
+      </c>
+      <c r="K7"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="10">
+        <v>43803.9137384259</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8">
+        <v>932184137</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" t="s">
         <v>26</v>
       </c>
-      <c r="I5" t="s">
-        <v>27</v>
-      </c>
-      <c r="J5" t="b">
-        <v>1</v>
-      </c>
-      <c r="K5"/>
+      <c r="J8" t="b">
+        <v>1</v>
+      </c>
+      <c r="K8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>